<commit_message>
Se cambio un dato del DS
</commit_message>
<xml_diff>
--- a/RxDemoDesktop/TC01_DS.xlsx
+++ b/RxDemoDesktop/TC01_DS.xlsx
@@ -57,12 +57,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>Esteban</t>
-  </si>
-  <si>
-    <t>Quito</t>
-  </si>
-  <si>
     <t>Office</t>
   </si>
   <si>
@@ -70,6 +64,12 @@
   </si>
   <si>
     <t>Marketing</t>
+  </si>
+  <si>
+    <t>Harry</t>
+  </si>
+  <si>
+    <t>Plotter</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,13 +469,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
       </c>
       <c r="D4">
         <v>32</v>
@@ -486,13 +486,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <v>60</v>

</xml_diff>